<commit_message>
permisos a carpeta de photos
</commit_message>
<xml_diff>
--- a/public/ReportOut.xlsx
+++ b/public/ReportOut.xlsx
@@ -20,6 +20,7 @@
     <definedName name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" localSheetId="0">'CR6 - 5.6'!$A$1:$AR$81</definedName>
     <definedName name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" localSheetId="0">'CR6 - 5.6'!$A$1:$AR$81</definedName>
     <definedName name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" localSheetId="0">'CR6 - 5.6'!$A$1:$AR$81</definedName>
+    <definedName name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" localSheetId="0">'CR6 - 5.6'!$A$1:$AR$81</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'CR6 - 5.6'!$A$1:$AR$81</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -68,7 +69,7 @@
     <t>Sistema bloqueado:</t>
   </si>
   <si>
-    <t>Agua Vapor</t>
+    <t>Vapor</t>
   </si>
   <si>
     <t>Ito Planta Turno día:</t>
@@ -158,6 +159,12 @@
     <t>Otro6</t>
   </si>
   <si>
+    <t>Corte de Caps</t>
+  </si>
+  <si>
+    <t>20 June, 2017, 3:36 pm</t>
+  </si>
+  <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
   </si>
   <si>
@@ -170,22 +177,46 @@
     <t>1.-</t>
   </si>
   <si>
+    <t>Marcado de Caps 3: Hola</t>
+  </si>
+  <si>
     <t>2.-</t>
+  </si>
+  <si>
+    <t>Marcado de Caps: Pf</t>
   </si>
   <si>
     <t>3.-</t>
   </si>
   <si>
+    <t>Otro3: Pf</t>
+  </si>
+  <si>
     <t>REGISTRO FOTOGRÁFICO</t>
   </si>
   <si>
+    <t>Otro4: Pf</t>
+  </si>
+  <si>
     <t>Foto 1:</t>
+  </si>
+  <si>
+    <t>Otro5: Pf</t>
   </si>
   <si>
     <t>Foto 2:</t>
   </si>
   <si>
     <t>Foto 3:</t>
+  </si>
+  <si>
+    <t>Otro6: Pf</t>
+  </si>
+  <si>
+    <t>Asusg</t>
+  </si>
+  <si>
+    <t>leyenda 2</t>
   </si>
 </sst>
 </file>
@@ -1017,9 +1048,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1343025" cy="647700"/>
     <xdr:pic>
@@ -1047,9 +1078,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2447925" cy="542925"/>
     <xdr:pic>
@@ -1077,7 +1108,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
@@ -1107,9 +1138,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1838325" cy="561975"/>
     <xdr:pic>
@@ -1136,15 +1167,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>7143750</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="5" name="Foto Trabajo 1" descr="Trabajo 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1166,15 +1197,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3333750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9048750</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="6" name="Foto Trabajo 2" descr="Trabajo 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1196,15 +1227,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5715000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9048750</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="7" name="Foto Trabajo 3" descr="Trabajo 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1226,15 +1257,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>10001250</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="8" name="Foto Trabajo 4" descr="Trabajo 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1256,15 +1287,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4762500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>10001250</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="9" name="Foto Trabajo 5" descr="Trabajo 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1286,15 +1317,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5715000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>10001250</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="2228850"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="10" name="Foto Trabajo 6" descr="Trabajo 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1612,7 +1643,7 @@
   <dimension ref="A1:AMK80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AT12" sqref="AT12"/>
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1631,7 +1662,7 @@
     <col min="12" max="12" width="3.42914979757085" customWidth="true" style="1"/>
     <col min="13" max="13" width="3.42914979757085" customWidth="true" style="1"/>
     <col min="14" max="14" width="3.42914979757085" customWidth="true" style="1"/>
-    <col min="15" max="15" width="3.42914979757085" customWidth="true" style="1"/>
+    <col min="15" max="15" width="22.2955465587045" customWidth="true" style="1"/>
     <col min="16" max="16" width="3.42914979757085" customWidth="true" style="1"/>
     <col min="17" max="17" width="3.42914979757085" customWidth="true" style="1"/>
     <col min="18" max="18" width="3.42914979757085" customWidth="true" style="1"/>
@@ -2645,7 +2676,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1025" customHeight="1" ht="15" s="2" customFormat="1">
-      <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6841,6 +6871,7 @@
       <c r="AM6" s="10"/>
       <c r="AN6" s="10"/>
       <c r="AO6" s="10"/>
+      <c r="AP6"/>
       <c r="AQ6" s="11"/>
       <c r="AR6"/>
       <c r="AS6"/>
@@ -21272,6 +21303,39 @@
       <c r="AO20" s="42"/>
       <c r="AP20" s="42"/>
       <c r="AQ20" s="42"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
+      <c r="BU20"/>
+      <c r="BV20"/>
+      <c r="BW20"/>
+      <c r="BX20"/>
       <c r="BY20"/>
       <c r="BZ20"/>
       <c r="CA20"/>
@@ -22273,6 +22337,39 @@
       <c r="AO21" s="46"/>
       <c r="AP21" s="46"/>
       <c r="AQ21" s="46"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+      <c r="AT21"/>
+      <c r="AU21"/>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21"/>
+      <c r="AY21"/>
+      <c r="AZ21"/>
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+      <c r="BE21"/>
+      <c r="BF21"/>
+      <c r="BG21"/>
+      <c r="BH21"/>
+      <c r="BI21"/>
+      <c r="BJ21"/>
+      <c r="BK21"/>
+      <c r="BL21"/>
+      <c r="BM21"/>
+      <c r="BN21"/>
+      <c r="BO21"/>
+      <c r="BP21"/>
+      <c r="BQ21"/>
+      <c r="BR21"/>
+      <c r="BS21"/>
+      <c r="BT21"/>
+      <c r="BU21"/>
+      <c r="BV21"/>
+      <c r="BW21"/>
+      <c r="BX21"/>
       <c r="BY21"/>
       <c r="BZ21"/>
       <c r="CA21"/>
@@ -23223,6 +23320,7 @@
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="15">
+      <c r="A22"/>
       <c r="B22" s="43"/>
       <c r="C22" s="44"/>
       <c r="D22" s="39"/>
@@ -23273,6 +23371,39 @@
       <c r="AO22" s="42"/>
       <c r="AP22" s="42"/>
       <c r="AQ22" s="42"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
+      <c r="BG22"/>
+      <c r="BH22"/>
+      <c r="BI22"/>
+      <c r="BJ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
+      <c r="BM22"/>
+      <c r="BN22"/>
+      <c r="BO22"/>
+      <c r="BP22"/>
+      <c r="BQ22"/>
+      <c r="BR22"/>
+      <c r="BS22"/>
+      <c r="BT22"/>
+      <c r="BU22"/>
+      <c r="BV22"/>
+      <c r="BW22"/>
+      <c r="BX22"/>
       <c r="BY22"/>
       <c r="BZ22"/>
       <c r="CA22"/>
@@ -24223,6 +24354,7 @@
       <c r="AMJ22"/>
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="15">
+      <c r="A23"/>
       <c r="B23" s="43"/>
       <c r="C23" s="44"/>
       <c r="D23" s="39"/>
@@ -24273,6 +24405,39 @@
       <c r="AO23" s="42"/>
       <c r="AP23" s="42"/>
       <c r="AQ23" s="42"/>
+      <c r="AR23"/>
+      <c r="AS23"/>
+      <c r="AT23"/>
+      <c r="AU23"/>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
+      <c r="BG23"/>
+      <c r="BH23"/>
+      <c r="BI23"/>
+      <c r="BJ23"/>
+      <c r="BK23"/>
+      <c r="BL23"/>
+      <c r="BM23"/>
+      <c r="BN23"/>
+      <c r="BO23"/>
+      <c r="BP23"/>
+      <c r="BQ23"/>
+      <c r="BR23"/>
+      <c r="BS23"/>
+      <c r="BT23"/>
+      <c r="BU23"/>
+      <c r="BV23"/>
+      <c r="BW23"/>
+      <c r="BX23"/>
       <c r="BY23"/>
       <c r="BZ23"/>
       <c r="CA23"/>
@@ -25443,6 +25608,38 @@
       <c r="AP26" s="46"/>
       <c r="AQ26" s="46"/>
       <c r="AR26" s="10"/>
+      <c r="AS26"/>
+      <c r="AT26"/>
+      <c r="AU26"/>
+      <c r="AV26"/>
+      <c r="AW26"/>
+      <c r="AX26"/>
+      <c r="AY26"/>
+      <c r="AZ26"/>
+      <c r="BA26"/>
+      <c r="BB26"/>
+      <c r="BC26"/>
+      <c r="BD26"/>
+      <c r="BE26"/>
+      <c r="BF26"/>
+      <c r="BG26"/>
+      <c r="BH26"/>
+      <c r="BI26"/>
+      <c r="BJ26"/>
+      <c r="BK26"/>
+      <c r="BL26"/>
+      <c r="BM26"/>
+      <c r="BN26"/>
+      <c r="BO26"/>
+      <c r="BP26"/>
+      <c r="BQ26"/>
+      <c r="BR26"/>
+      <c r="BS26"/>
+      <c r="BT26"/>
+      <c r="BU26"/>
+      <c r="BV26"/>
+      <c r="BW26"/>
+      <c r="BX26"/>
       <c r="BY26"/>
       <c r="BZ26"/>
       <c r="CA26"/>
@@ -26397,7 +26594,9 @@
       <c r="B27" s="43"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="E27" s="39" t="s">
+        <v>43</v>
+      </c>
       <c r="F27" s="39"/>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
@@ -26420,19 +26619,25 @@
       <c r="Y27" s="39"/>
       <c r="Z27" s="39"/>
       <c r="AA27" s="39"/>
-      <c r="AB27" s="47"/>
+      <c r="AB27" s="47" t="s">
+        <v>44</v>
+      </c>
       <c r="AC27" s="47"/>
       <c r="AD27" s="47"/>
       <c r="AE27" s="47"/>
       <c r="AF27" s="47"/>
       <c r="AG27" s="47"/>
-      <c r="AH27" s="47"/>
+      <c r="AH27" s="47" t="s">
+        <v>44</v>
+      </c>
       <c r="AI27" s="47"/>
       <c r="AJ27" s="47"/>
       <c r="AK27" s="47"/>
       <c r="AL27" s="47"/>
       <c r="AM27" s="47"/>
-      <c r="AN27" s="42"/>
+      <c r="AN27" s="42">
+        <v>88</v>
+      </c>
       <c r="AO27" s="42"/>
       <c r="AP27" s="42"/>
       <c r="AQ27" s="42"/>
@@ -27463,6 +27668,38 @@
       <c r="AP28" s="46"/>
       <c r="AQ28" s="46"/>
       <c r="AR28" s="10"/>
+      <c r="AS28"/>
+      <c r="AT28"/>
+      <c r="AU28"/>
+      <c r="AV28"/>
+      <c r="AW28"/>
+      <c r="AX28"/>
+      <c r="AY28"/>
+      <c r="AZ28"/>
+      <c r="BA28"/>
+      <c r="BB28"/>
+      <c r="BC28"/>
+      <c r="BD28"/>
+      <c r="BE28"/>
+      <c r="BF28"/>
+      <c r="BG28"/>
+      <c r="BH28"/>
+      <c r="BI28"/>
+      <c r="BJ28"/>
+      <c r="BK28"/>
+      <c r="BL28"/>
+      <c r="BM28"/>
+      <c r="BN28"/>
+      <c r="BO28"/>
+      <c r="BP28"/>
+      <c r="BQ28"/>
+      <c r="BR28"/>
+      <c r="BS28"/>
+      <c r="BT28"/>
+      <c r="BU28"/>
+      <c r="BV28"/>
+      <c r="BW28"/>
+      <c r="BX28"/>
       <c r="BY28"/>
       <c r="BZ28"/>
       <c r="CA28"/>
@@ -28457,6 +28694,38 @@
       <c r="AP29" s="42"/>
       <c r="AQ29" s="42"/>
       <c r="AR29" s="10"/>
+      <c r="AS29"/>
+      <c r="AT29"/>
+      <c r="AU29"/>
+      <c r="AV29"/>
+      <c r="AW29"/>
+      <c r="AX29"/>
+      <c r="AY29"/>
+      <c r="AZ29"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+      <c r="BE29"/>
+      <c r="BF29"/>
+      <c r="BG29"/>
+      <c r="BH29"/>
+      <c r="BI29"/>
+      <c r="BJ29"/>
+      <c r="BK29"/>
+      <c r="BL29"/>
+      <c r="BM29"/>
+      <c r="BN29"/>
+      <c r="BO29"/>
+      <c r="BP29"/>
+      <c r="BQ29"/>
+      <c r="BR29"/>
+      <c r="BS29"/>
+      <c r="BT29"/>
+      <c r="BU29"/>
+      <c r="BV29"/>
+      <c r="BW29"/>
+      <c r="BX29"/>
       <c r="BY29"/>
       <c r="BZ29"/>
       <c r="CA29"/>
@@ -29451,6 +29720,38 @@
       <c r="AP30" s="42"/>
       <c r="AQ30" s="42"/>
       <c r="AR30" s="10"/>
+      <c r="AS30"/>
+      <c r="AT30"/>
+      <c r="AU30"/>
+      <c r="AV30"/>
+      <c r="AW30"/>
+      <c r="AX30"/>
+      <c r="AY30"/>
+      <c r="AZ30"/>
+      <c r="BA30"/>
+      <c r="BB30"/>
+      <c r="BC30"/>
+      <c r="BD30"/>
+      <c r="BE30"/>
+      <c r="BF30"/>
+      <c r="BG30"/>
+      <c r="BH30"/>
+      <c r="BI30"/>
+      <c r="BJ30"/>
+      <c r="BK30"/>
+      <c r="BL30"/>
+      <c r="BM30"/>
+      <c r="BN30"/>
+      <c r="BO30"/>
+      <c r="BP30"/>
+      <c r="BQ30"/>
+      <c r="BR30"/>
+      <c r="BS30"/>
+      <c r="BT30"/>
+      <c r="BU30"/>
+      <c r="BV30"/>
+      <c r="BW30"/>
+      <c r="BX30"/>
       <c r="BY30"/>
       <c r="BZ30"/>
       <c r="CA30"/>
@@ -30445,6 +30746,38 @@
       <c r="AP31" s="46"/>
       <c r="AQ31" s="46"/>
       <c r="AR31" s="10"/>
+      <c r="AS31"/>
+      <c r="AT31"/>
+      <c r="AU31"/>
+      <c r="AV31"/>
+      <c r="AW31"/>
+      <c r="AX31"/>
+      <c r="AY31"/>
+      <c r="AZ31"/>
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+      <c r="BE31"/>
+      <c r="BF31"/>
+      <c r="BG31"/>
+      <c r="BH31"/>
+      <c r="BI31"/>
+      <c r="BJ31"/>
+      <c r="BK31"/>
+      <c r="BL31"/>
+      <c r="BM31"/>
+      <c r="BN31"/>
+      <c r="BO31"/>
+      <c r="BP31"/>
+      <c r="BQ31"/>
+      <c r="BR31"/>
+      <c r="BS31"/>
+      <c r="BT31"/>
+      <c r="BU31"/>
+      <c r="BV31"/>
+      <c r="BW31"/>
+      <c r="BX31"/>
       <c r="BY31"/>
       <c r="BZ31"/>
       <c r="CA31"/>
@@ -31439,6 +31772,38 @@
       <c r="AP32" s="46"/>
       <c r="AQ32" s="46"/>
       <c r="AR32" s="10"/>
+      <c r="AS32"/>
+      <c r="AT32"/>
+      <c r="AU32"/>
+      <c r="AV32"/>
+      <c r="AW32"/>
+      <c r="AX32"/>
+      <c r="AY32"/>
+      <c r="AZ32"/>
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+      <c r="BE32"/>
+      <c r="BF32"/>
+      <c r="BG32"/>
+      <c r="BH32"/>
+      <c r="BI32"/>
+      <c r="BJ32"/>
+      <c r="BK32"/>
+      <c r="BL32"/>
+      <c r="BM32"/>
+      <c r="BN32"/>
+      <c r="BO32"/>
+      <c r="BP32"/>
+      <c r="BQ32"/>
+      <c r="BR32"/>
+      <c r="BS32"/>
+      <c r="BT32"/>
+      <c r="BU32"/>
+      <c r="BV32"/>
+      <c r="BW32"/>
+      <c r="BX32"/>
       <c r="BY32"/>
       <c r="BZ32"/>
       <c r="CA32"/>
@@ -42651,7 +43016,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="10"/>
       <c r="B43" s="55" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
@@ -43679,7 +44044,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="10"/>
       <c r="B44" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -43716,7 +44081,7 @@
       <c r="AI44" s="24"/>
       <c r="AJ44" s="24"/>
       <c r="AK44" s="25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AL44" s="25"/>
       <c r="AM44" s="25"/>
@@ -44710,9 +45075,11 @@
       <c r="A45" s="10"/>
       <c r="B45" s="56"/>
       <c r="C45" s="57" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
-      <c r="D45" s="57"/>
+      <c r="D45" s="57" t="s">
+        <v>49</v>
+      </c>
       <c r="E45" s="57"/>
       <c r="F45" s="58"/>
       <c r="G45" s="58"/>
@@ -45738,9 +46105,11 @@
       <c r="A46" s="10"/>
       <c r="B46" s="56"/>
       <c r="C46" s="57" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
-      <c r="D46" s="57"/>
+      <c r="D46" s="57" t="s">
+        <v>51</v>
+      </c>
       <c r="E46" s="57"/>
       <c r="F46" s="58"/>
       <c r="G46" s="58"/>
@@ -46766,9 +47135,11 @@
       <c r="A47" s="10"/>
       <c r="B47" s="61"/>
       <c r="C47" s="62" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
-      <c r="D47" s="62"/>
+      <c r="D47" s="62" t="s">
+        <v>53</v>
+      </c>
       <c r="E47" s="62"/>
       <c r="F47" s="62"/>
       <c r="G47" s="62"/>
@@ -47793,10 +48164,12 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="10"/>
       <c r="B48" s="65" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
+      <c r="D48" s="65" t="s">
+        <v>55</v>
+      </c>
       <c r="E48" s="65"/>
       <c r="F48" s="65"/>
       <c r="G48" s="65"/>
@@ -48821,10 +49194,12 @@
     <row r="49" spans="1:1025" customHeight="1" ht="15">
       <c r="A49" s="10"/>
       <c r="B49" s="66" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C49" s="66"/>
-      <c r="D49" s="67"/>
+      <c r="D49" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E49" s="67"/>
       <c r="F49" s="67"/>
       <c r="G49" s="67"/>
@@ -48837,7 +49212,7 @@
       <c r="N49" s="67"/>
       <c r="O49" s="67"/>
       <c r="P49" s="68" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="Q49" s="68"/>
       <c r="R49" s="67"/>
@@ -48853,7 +49228,7 @@
       <c r="AB49" s="67"/>
       <c r="AC49" s="67"/>
       <c r="AD49" s="68" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AE49" s="68"/>
       <c r="AF49" s="67"/>
@@ -49854,7 +50229,9 @@
       <c r="A50" s="10"/>
       <c r="B50" s="69"/>
       <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
+      <c r="D50" s="69" t="s">
+        <v>60</v>
+      </c>
       <c r="E50" s="69"/>
       <c r="F50" s="69"/>
       <c r="G50" s="69"/>
@@ -51906,7 +52283,9 @@
       <c r="A52" s="10"/>
       <c r="B52" s="69"/>
       <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
+      <c r="D52" s="69" t="s">
+        <v>61</v>
+      </c>
       <c r="E52" s="69"/>
       <c r="F52" s="69"/>
       <c r="G52" s="69"/>
@@ -51920,7 +52299,9 @@
       <c r="O52" s="69"/>
       <c r="P52" s="70"/>
       <c r="Q52" s="70"/>
-      <c r="R52" s="70"/>
+      <c r="R52" s="70" t="s">
+        <v>62</v>
+      </c>
       <c r="S52" s="70"/>
       <c r="T52" s="70"/>
       <c r="U52" s="70"/>
@@ -51934,7 +52315,9 @@
       <c r="AC52" s="70"/>
       <c r="AD52" s="71"/>
       <c r="AE52" s="71"/>
-      <c r="AF52" s="71"/>
+      <c r="AF52" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="AG52" s="71"/>
       <c r="AH52" s="71"/>
       <c r="AI52" s="71"/>
@@ -62209,6 +62592,45 @@
     <row r="63" spans="1:1025" customHeight="1" ht="15">
       <c r="A63"/>
       <c r="B63" s="72"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63"/>
+      <c r="Y63"/>
+      <c r="Z63"/>
+      <c r="AA63"/>
+      <c r="AB63"/>
+      <c r="AC63"/>
+      <c r="AD63"/>
+      <c r="AE63"/>
+      <c r="AF63"/>
+      <c r="AG63"/>
+      <c r="AH63"/>
+      <c r="AI63"/>
+      <c r="AJ63"/>
+      <c r="AK63"/>
+      <c r="AL63"/>
+      <c r="AM63"/>
+      <c r="AN63"/>
+      <c r="AO63"/>
       <c r="AP63" s="10"/>
       <c r="AQ63" s="73"/>
       <c r="AR63"/>
@@ -63196,7 +63618,7 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="66" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C64" s="66"/>
       <c r="D64" s="67"/>
@@ -63212,7 +63634,7 @@
       <c r="N64" s="67"/>
       <c r="O64" s="67"/>
       <c r="P64" s="68" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="Q64" s="68"/>
       <c r="R64" s="67"/>
@@ -63228,7 +63650,7 @@
       <c r="AB64" s="67"/>
       <c r="AC64" s="67"/>
       <c r="AD64" s="68" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AE64" s="68"/>
       <c r="AF64" s="74"/>
@@ -66281,7 +66703,9 @@
       <c r="A67"/>
       <c r="B67" s="69"/>
       <c r="C67" s="69"/>
-      <c r="D67" s="69"/>
+      <c r="D67" s="69" t="s">
+        <v>62</v>
+      </c>
       <c r="E67" s="69"/>
       <c r="F67" s="69"/>
       <c r="G67" s="69"/>
@@ -66295,7 +66719,9 @@
       <c r="O67" s="69"/>
       <c r="P67" s="70"/>
       <c r="Q67" s="70"/>
-      <c r="R67" s="70"/>
+      <c r="R67" s="70" t="s">
+        <v>62</v>
+      </c>
       <c r="S67" s="70"/>
       <c r="T67" s="70"/>
       <c r="U67" s="70"/>
@@ -66309,7 +66735,9 @@
       <c r="AC67" s="70"/>
       <c r="AD67" s="71"/>
       <c r="AE67" s="71"/>
-      <c r="AF67" s="71"/>
+      <c r="AF67" s="71" t="s">
+        <v>62</v>
+      </c>
       <c r="AG67" s="71"/>
       <c r="AH67" s="71"/>
       <c r="AI67" s="71"/>
@@ -76583,10 +77011,51 @@
     </row>
     <row r="78" spans="1:1025" customHeight="1" ht="15">
       <c r="B78" s="72"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
+      <c r="R78"/>
+      <c r="S78"/>
+      <c r="T78"/>
+      <c r="U78"/>
+      <c r="V78"/>
+      <c r="W78"/>
+      <c r="X78"/>
+      <c r="Y78"/>
+      <c r="Z78"/>
+      <c r="AA78"/>
+      <c r="AB78"/>
+      <c r="AC78"/>
+      <c r="AD78"/>
+      <c r="AE78"/>
+      <c r="AF78"/>
+      <c r="AG78"/>
+      <c r="AH78"/>
+      <c r="AI78"/>
+      <c r="AJ78"/>
+      <c r="AK78"/>
+      <c r="AL78"/>
+      <c r="AM78"/>
+      <c r="AN78"/>
+      <c r="AO78"/>
+      <c r="AP78"/>
       <c r="AQ78" s="11"/>
     </row>
     <row r="79" spans="1:1025" customHeight="1" ht="15">
       <c r="B79" s="72"/>
+      <c r="C79"/>
       <c r="D79" s="10"/>
       <c r="E79" s="39"/>
       <c r="F79" s="39"/>
@@ -76622,6 +77091,9 @@
       <c r="AJ79" s="39"/>
       <c r="AK79" s="39"/>
       <c r="AL79" s="10"/>
+      <c r="AM79"/>
+      <c r="AN79"/>
+      <c r="AO79"/>
       <c r="AP79" s="75">
         <v>13</v>
       </c>

</xml_diff>